<commit_message>
set parent material custom user input
</commit_message>
<xml_diff>
--- a/MISLAND/data/summary_table_ldn_annual.xlsx
+++ b/MISLAND/data/summary_table_ldn_annual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\trends.earth\MISLAND\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C90928-64F9-4905-9A34-66CBE409B9A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20FD141-D8A7-401F-A2B8-CFF62FC618DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
@@ -19,19 +19,11 @@
     <sheet name="Land cover" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="81">
   <si>
     <t>Land area with improved productivity:</t>
   </si>
@@ -90,18 +82,9 @@
     <t>No data</t>
   </si>
   <si>
-    <t>Trends.Earth SDG 15.3.1 summary table</t>
-  </si>
-  <si>
     <t>For more information on Trends.Earth, see http://trends.earth, or contact the team at trends.earth@conservation.org.</t>
   </si>
   <si>
-    <t>Trends.Earth productivity summary table</t>
-  </si>
-  <si>
-    <t>Trends.Earth soil organic carbon summary table</t>
-  </si>
-  <si>
     <t>Land area with improved soil organic carbon:</t>
   </si>
   <si>
@@ -114,9 +97,6 @@
     <t>Land area with no data for soil organic carbon:</t>
   </si>
   <si>
-    <t>Trends.Earth land cover summary table</t>
-  </si>
-  <si>
     <t>Land area with improved land cover:</t>
   </si>
   <si>
@@ -274,6 +254,18 @@
   </si>
   <si>
     <t>Summary by percent of land area (%)</t>
+  </si>
+  <si>
+    <t>Misland SDG 15.3.1 summary table</t>
+  </si>
+  <si>
+    <t>Misland productivity summary table</t>
+  </si>
+  <si>
+    <t>Misland soil organic carbon summary table</t>
+  </si>
+  <si>
+    <t>Misland land cover summary table</t>
   </si>
 </sst>
 </file>
@@ -281,9 +273,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -902,7 +894,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1011,10 +1003,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1034,19 +1026,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1094,89 +1086,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="9" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="17" fillId="8" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="17" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="17" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="17" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="9" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1184,21 +1182,60 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1208,57 +1245,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="12" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1272,59 +1322,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1336,14 +1334,8 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1707,28 +1699,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" style="34" customWidth="1"/>
-    <col min="2" max="2" width="14.53125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="14.73046875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="16.46484375" style="35" customWidth="1"/>
-    <col min="6" max="6" width="6.796875" style="35" customWidth="1"/>
-    <col min="7" max="7" width="14.53125" style="65" customWidth="1"/>
-    <col min="8" max="8" width="17.796875" style="67" customWidth="1"/>
-    <col min="9" max="9" width="14.73046875" style="67" customWidth="1"/>
-    <col min="10" max="10" width="16.46484375" style="67" customWidth="1"/>
-    <col min="11" max="16384" width="9.19921875" style="34"/>
+    <col min="1" max="1" width="8.77734375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="35" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" style="35" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="65" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="67" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="67" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="67" customWidth="1"/>
+    <col min="11" max="16384" width="9.21875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="12"/>
@@ -1740,24 +1732,24 @@
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="16.899999999999999" x14ac:dyDescent="0.5">
-      <c r="A3" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-    </row>
-    <row r="4" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A3" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+    </row>
+    <row r="4" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -1767,41 +1759,41 @@
       <c r="I4" s="68"/>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="1:10" s="39" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" s="39" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="42"/>
-      <c r="B5" s="106" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
+      <c r="B5" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="70"/>
-      <c r="G5" s="106" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-    </row>
-    <row r="6" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G5" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+    </row>
+    <row r="6" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="71"/>
-      <c r="B6" s="114" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="124">
+      <c r="B6" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="118">
         <v>34.799999999999997</v>
       </c>
       <c r="D6" s="76">
         <v>15.5</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F6" s="72"/>
-      <c r="G6" s="114" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="115">
+      <c r="G6" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="109">
         <f>C6/C14</f>
         <v>0.26008968609865468</v>
       </c>
@@ -1810,50 +1802,50 @@
         <v>0.11584454409566516</v>
       </c>
       <c r="J6" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="60" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="60" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="71"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="125"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="78">
         <f>C6-D6</f>
         <v>19.299999999999997</v>
       </c>
       <c r="E7" s="79" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F7" s="64"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="116"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="110"/>
       <c r="I7" s="92">
         <f t="shared" ref="I7:I13" si="0">D7/$C$14</f>
         <v>0.14424514200298949</v>
       </c>
       <c r="J7" s="79" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="55" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="55" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="71"/>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="121">
+      <c r="C8" s="115">
         <v>94.3</v>
       </c>
       <c r="D8" s="80">
         <v>70.400000000000006</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="64"/>
-      <c r="G8" s="101" t="s">
+      <c r="G8" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="118">
+      <c r="H8" s="112">
         <f>C8/C14</f>
         <v>0.70478325859491775</v>
       </c>
@@ -1862,71 +1854,71 @@
         <v>0.52615844544095669</v>
       </c>
       <c r="J8" s="81" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="55" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="55" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
-      <c r="B9" s="117"/>
-      <c r="C9" s="122"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="116"/>
       <c r="D9" s="82">
         <v>15</v>
       </c>
       <c r="E9" s="83" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F9" s="64"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="119"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="113"/>
       <c r="I9" s="94">
         <f t="shared" si="0"/>
         <v>0.11210762331838564</v>
       </c>
       <c r="J9" s="83" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="123"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="117"/>
       <c r="D10" s="84">
         <f>C8-D9-D8</f>
         <v>8.8999999999999915</v>
       </c>
       <c r="E10" s="85" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F10" s="72"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="120"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="114"/>
       <c r="I10" s="95">
         <f t="shared" si="0"/>
         <v>6.6517189835575419E-2</v>
       </c>
       <c r="J10" s="85" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="60" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="60" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="71"/>
-      <c r="B11" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="103">
+      <c r="B11" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="120">
         <v>3.4</v>
       </c>
       <c r="D11" s="86">
         <v>2</v>
       </c>
       <c r="E11" s="87" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F11" s="64"/>
-      <c r="G11" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="112">
+      <c r="G11" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="105">
         <f>C11/C14</f>
         <v>2.5411061285500743E-2</v>
       </c>
@@ -1935,32 +1927,32 @@
         <v>1.4947683109118086E-2</v>
       </c>
       <c r="J11" s="87" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="71"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="104"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="88">
         <f>C11-D11</f>
         <v>1.4</v>
       </c>
       <c r="E12" s="89" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" s="72"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="113"/>
+      <c r="G12" s="104"/>
+      <c r="H12" s="106"/>
       <c r="I12" s="97">
         <f t="shared" si="0"/>
         <v>1.0463378176382659E-2</v>
       </c>
       <c r="J12" s="89" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="71"/>
       <c r="B13" s="69" t="s">
         <v>18</v>
@@ -1991,10 +1983,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="72"/>
       <c r="B14" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="73">
         <f>SUM(C6:C13)</f>
@@ -2006,7 +1998,7 @@
       </c>
       <c r="F14" s="64"/>
       <c r="G14" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H14" s="100">
         <f>SUM(H6:H13)</f>
@@ -2017,7 +2009,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="72"/>
       <c r="B15" s="28"/>
       <c r="C15" s="73"/>
@@ -2029,68 +2021,68 @@
       <c r="I15" s="73"/>
       <c r="J15" s="67"/>
     </row>
-    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="65" customFormat="1" ht="35.200000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="105" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-    </row>
-    <row r="18" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="109"/>
-      <c r="J18" s="110"/>
-    </row>
-    <row r="20" spans="1:10" s="65" customFormat="1" ht="35.200000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="105" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="105"/>
-    </row>
-    <row r="21" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="109"/>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="110"/>
-    </row>
-    <row r="22" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="65" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="122" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+    </row>
+    <row r="18" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="125"/>
+    </row>
+    <row r="20" spans="1:10" s="65" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="122"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="122"/>
+      <c r="G20" s="122"/>
+      <c r="H20" s="122"/>
+      <c r="I20" s="122"/>
+      <c r="J20" s="122"/>
+    </row>
+    <row r="21" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="124"/>
+      <c r="C21" s="124"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="124"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="125"/>
+    </row>
+    <row r="22" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="67"/>
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
@@ -2099,35 +2091,35 @@
       <c r="I22" s="67"/>
       <c r="J22" s="67"/>
     </row>
-    <row r="23" spans="1:10" s="65" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-    </row>
-    <row r="24" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="109"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="110"/>
-    </row>
-    <row r="25" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" s="65" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="122"/>
+      <c r="H23" s="122"/>
+      <c r="I23" s="122"/>
+      <c r="J23" s="122"/>
+    </row>
+    <row r="24" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="124"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="124"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="125"/>
+    </row>
+    <row r="25" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="67"/>
       <c r="D25" s="67"/>
       <c r="E25" s="67"/>
@@ -2136,35 +2128,35 @@
       <c r="I25" s="67"/>
       <c r="J25" s="67"/>
     </row>
-    <row r="26" spans="1:10" s="65" customFormat="1" ht="35.200000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="105" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
-    </row>
-    <row r="27" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="110"/>
-    </row>
-    <row r="28" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" s="65" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="122" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122"/>
+    </row>
+    <row r="27" spans="1:10" s="65" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="125"/>
+    </row>
+    <row r="28" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="67"/>
       <c r="D28" s="67"/>
       <c r="E28" s="67"/>
@@ -2173,21 +2165,21 @@
       <c r="I28" s="67"/>
       <c r="J28" s="67"/>
     </row>
-    <row r="29" spans="1:10" s="66" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="107" t="s">
+    <row r="29" spans="1:10" s="66" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-    </row>
-    <row r="30" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="102"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+    </row>
+    <row r="30" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="67"/>
       <c r="D30" s="67"/>
       <c r="E30" s="67"/>
@@ -2196,22 +2188,29 @@
       <c r="I30" s="67"/>
       <c r="J30" s="67"/>
     </row>
-    <row r="31" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="107" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="107"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
+    <row r="31" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="102"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A21:J21"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="G11:G12"/>
@@ -2228,15 +2227,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="A17:J17"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A21:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2247,21 +2237,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" style="65"/>
-    <col min="2" max="2" width="8.73046875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" style="34" customWidth="1"/>
-    <col min="4" max="10" width="15.53125" style="35" customWidth="1"/>
-    <col min="11" max="11" width="15.53125" style="36" customWidth="1"/>
-    <col min="12" max="16384" width="9.19921875" style="34"/>
+    <col min="1" max="1" width="9.21875" style="65"/>
+    <col min="2" max="2" width="8.77734375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="34" customWidth="1"/>
+    <col min="4" max="10" width="15.5546875" style="35" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="36" customWidth="1"/>
+    <col min="12" max="16384" width="9.21875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="48" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:11" s="48" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C1" s="65"/>
       <c r="D1" s="65"/>
@@ -2273,7 +2265,7 @@
       <c r="J1" s="65"/>
       <c r="K1" s="65"/>
     </row>
-    <row r="2" spans="1:11" s="48" customFormat="1" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" s="48" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="65"/>
       <c r="B2" s="4"/>
       <c r="C2" s="65"/>
@@ -2286,44 +2278,44 @@
       <c r="J2" s="65"/>
       <c r="K2" s="65"/>
     </row>
-    <row r="3" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="129" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+    </row>
+    <row r="4" spans="1:11" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="65"/>
       <c r="C4" s="67"/>
       <c r="D4" s="67"/>
       <c r="E4" s="67"/>
       <c r="F4" s="42" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H4" s="67"/>
       <c r="I4" s="67"/>
       <c r="J4" s="68"/>
     </row>
-    <row r="5" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="65"/>
       <c r="C5" s="67"/>
       <c r="D5" s="67"/>
       <c r="E5" s="28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="40">
         <f>SUM(F6:F9)</f>
@@ -2337,7 +2329,7 @@
       <c r="I5" s="67"/>
       <c r="J5" s="68"/>
     </row>
-    <row r="6" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="65"/>
       <c r="C6" s="67"/>
@@ -2354,7 +2346,7 @@
       <c r="I6" s="67"/>
       <c r="J6" s="68"/>
     </row>
-    <row r="7" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="65"/>
       <c r="C7" s="67"/>
@@ -2371,7 +2363,7 @@
       <c r="I7" s="67"/>
       <c r="J7" s="68"/>
     </row>
-    <row r="8" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="65"/>
       <c r="C8" s="67"/>
@@ -2388,7 +2380,7 @@
       <c r="I8" s="67"/>
       <c r="J8" s="68"/>
     </row>
-    <row r="9" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="65"/>
       <c r="C9" s="67"/>
@@ -2405,7 +2397,7 @@
       <c r="I9" s="67"/>
       <c r="J9" s="68"/>
     </row>
-    <row r="10" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="65"/>
       <c r="B10" s="4"/>
       <c r="C10" s="65"/>
@@ -2418,22 +2410,22 @@
       <c r="J10" s="67"/>
       <c r="K10" s="68"/>
     </row>
-    <row r="11" spans="1:11" s="48" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="107" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="107"/>
-    </row>
-    <row r="12" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" s="48" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="102" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+    </row>
+    <row r="12" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
       <c r="B12" s="4"/>
       <c r="D12" s="46"/>
@@ -2445,28 +2437,28 @@
       <c r="J12" s="46"/>
       <c r="K12" s="47"/>
     </row>
-    <row r="13" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="130" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="128" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="128"/>
-      <c r="K13" s="128"/>
-    </row>
-    <row r="14" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="130"/>
+    <row r="13" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="152" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
+    </row>
+    <row r="14" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="152"/>
       <c r="C14" s="1"/>
       <c r="D14" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E14" s="134"/>
       <c r="F14" s="134"/>
@@ -2475,8 +2467,8 @@
       <c r="I14" s="134"/>
       <c r="J14" s="134"/>
     </row>
-    <row r="15" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="130"/>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="152"/>
       <c r="D15" s="59" t="s">
         <v>15</v>
       </c>
@@ -2493,7 +2485,7 @@
         <v>7</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>8</v>
@@ -2502,10 +2494,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="130"/>
-      <c r="B16" s="126" t="s">
-        <v>66</v>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="152"/>
+      <c r="B16" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C16" s="56" t="s">
         <v>15</v>
@@ -2522,9 +2514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="130"/>
-      <c r="B17" s="127"/>
+    <row r="17" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="152"/>
+      <c r="B17" s="128"/>
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
@@ -2540,9 +2532,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="130"/>
-      <c r="B18" s="127"/>
+    <row r="18" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="152"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
@@ -2558,9 +2550,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="130"/>
-      <c r="B19" s="127"/>
+    <row r="19" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="152"/>
+      <c r="B19" s="128"/>
       <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
@@ -2576,9 +2568,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="130"/>
-      <c r="B20" s="127"/>
+    <row r="20" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="152"/>
+      <c r="B20" s="128"/>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2594,11 +2586,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="130"/>
-      <c r="B21" s="127"/>
+    <row r="21" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="152"/>
+      <c r="B21" s="128"/>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2612,9 +2604,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="130"/>
-      <c r="B22" s="127"/>
+    <row r="22" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="152"/>
+      <c r="B22" s="128"/>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
@@ -2630,8 +2622,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="130"/>
+    <row r="23" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="152"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6" t="s">
         <v>9</v>
@@ -2669,28 +2661,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="131" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="135" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="135"/>
-      <c r="D25" s="135"/>
-      <c r="E25" s="135"/>
-      <c r="F25" s="135"/>
-      <c r="G25" s="135"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="135"/>
-      <c r="J25" s="135"/>
-      <c r="K25" s="135"/>
-    </row>
-    <row r="26" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="131"/>
+    <row r="25" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="153" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="155" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="155"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="155"/>
+      <c r="G25" s="155"/>
+      <c r="H25" s="155"/>
+      <c r="I25" s="155"/>
+      <c r="J25" s="155"/>
+      <c r="K25" s="155"/>
+    </row>
+    <row r="26" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="153"/>
       <c r="C26" s="1"/>
       <c r="D26" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E26" s="134"/>
       <c r="F26" s="134"/>
@@ -2699,8 +2691,8 @@
       <c r="I26" s="134"/>
       <c r="J26" s="134"/>
     </row>
-    <row r="27" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="131"/>
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="153"/>
       <c r="D27" s="58" t="s">
         <v>15</v>
       </c>
@@ -2717,7 +2709,7 @@
         <v>7</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>8</v>
@@ -2726,10 +2718,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="131"/>
-      <c r="B28" s="126" t="s">
-        <v>66</v>
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="153"/>
+      <c r="B28" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C28" s="56" t="s">
         <v>15</v>
@@ -2746,9 +2738,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="131"/>
-      <c r="B29" s="127"/>
+    <row r="29" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="153"/>
+      <c r="B29" s="128"/>
       <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
@@ -2764,9 +2756,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="131"/>
-      <c r="B30" s="127"/>
+    <row r="30" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="153"/>
+      <c r="B30" s="128"/>
       <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2782,9 +2774,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="131"/>
-      <c r="B31" s="127"/>
+    <row r="31" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="153"/>
+      <c r="B31" s="128"/>
       <c r="C31" s="2" t="s">
         <v>6</v>
       </c>
@@ -2800,9 +2792,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="131"/>
-      <c r="B32" s="127"/>
+    <row r="32" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="153"/>
+      <c r="B32" s="128"/>
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
@@ -2818,11 +2810,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="131"/>
-      <c r="B33" s="127"/>
+    <row r="33" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="153"/>
+      <c r="B33" s="128"/>
       <c r="C33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -2836,9 +2828,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="131"/>
-      <c r="B34" s="127"/>
+    <row r="34" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="153"/>
+      <c r="B34" s="128"/>
       <c r="C34" s="2" t="s">
         <v>8</v>
       </c>
@@ -2854,8 +2846,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="131"/>
+    <row r="35" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="153"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6" t="s">
         <v>9</v>
@@ -2893,28 +2885,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="155" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="137" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="138"/>
-      <c r="D37" s="139"/>
-      <c r="E37" s="139"/>
-      <c r="F37" s="139"/>
-      <c r="G37" s="139"/>
-      <c r="H37" s="139"/>
-      <c r="I37" s="139"/>
-      <c r="J37" s="139"/>
-      <c r="K37" s="140"/>
-    </row>
-    <row r="38" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="155"/>
+    <row r="37" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="157" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="129" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="130"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="131"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="131"/>
+      <c r="K37" s="132"/>
+    </row>
+    <row r="38" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="157"/>
       <c r="C38" s="1"/>
       <c r="D38" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E38" s="134"/>
       <c r="F38" s="134"/>
@@ -2923,8 +2915,8 @@
       <c r="I38" s="134"/>
       <c r="J38" s="134"/>
     </row>
-    <row r="39" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="155"/>
+    <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="157"/>
       <c r="D39" s="58" t="s">
         <v>15</v>
       </c>
@@ -2941,7 +2933,7 @@
         <v>7</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>8</v>
@@ -2950,10 +2942,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="155"/>
-      <c r="B40" s="126" t="s">
-        <v>66</v>
+    <row r="40" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="157"/>
+      <c r="B40" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C40" s="56" t="s">
         <v>15</v>
@@ -2970,9 +2962,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="155"/>
-      <c r="B41" s="127"/>
+    <row r="41" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="157"/>
+      <c r="B41" s="128"/>
       <c r="C41" s="2" t="s">
         <v>4</v>
       </c>
@@ -2988,9 +2980,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="155"/>
-      <c r="B42" s="127"/>
+    <row r="42" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="157"/>
+      <c r="B42" s="128"/>
       <c r="C42" s="2" t="s">
         <v>5</v>
       </c>
@@ -3006,9 +2998,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="155"/>
-      <c r="B43" s="127"/>
+    <row r="43" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="157"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="2" t="s">
         <v>6</v>
       </c>
@@ -3024,9 +3016,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="155"/>
-      <c r="B44" s="127"/>
+    <row r="44" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="157"/>
+      <c r="B44" s="128"/>
       <c r="C44" s="2" t="s">
         <v>7</v>
       </c>
@@ -3042,11 +3034,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="155"/>
-      <c r="B45" s="127"/>
+    <row r="45" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="157"/>
+      <c r="B45" s="128"/>
       <c r="C45" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="23"/>
@@ -3060,9 +3052,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="155"/>
-      <c r="B46" s="127"/>
+    <row r="46" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="157"/>
+      <c r="B46" s="128"/>
       <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
@@ -3078,8 +3070,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="155"/>
+    <row r="47" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="157"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6" t="s">
         <v>9</v>
@@ -3117,28 +3109,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="156" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="141" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="142"/>
-      <c r="D49" s="143"/>
-      <c r="E49" s="143"/>
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="143"/>
-      <c r="I49" s="143"/>
-      <c r="J49" s="143"/>
-      <c r="K49" s="144"/>
-    </row>
-    <row r="50" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="156"/>
+    <row r="49" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="158" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="135" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="136"/>
+      <c r="D49" s="137"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="137"/>
+      <c r="G49" s="137"/>
+      <c r="H49" s="137"/>
+      <c r="I49" s="137"/>
+      <c r="J49" s="137"/>
+      <c r="K49" s="138"/>
+    </row>
+    <row r="50" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="158"/>
       <c r="C50" s="1"/>
       <c r="D50" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E50" s="134"/>
       <c r="F50" s="134"/>
@@ -3147,8 +3139,8 @@
       <c r="I50" s="134"/>
       <c r="J50" s="134"/>
     </row>
-    <row r="51" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="156"/>
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="158"/>
       <c r="D51" s="58" t="s">
         <v>15</v>
       </c>
@@ -3165,7 +3157,7 @@
         <v>7</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J51" s="7" t="s">
         <v>8</v>
@@ -3174,10 +3166,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A52" s="156"/>
-      <c r="B52" s="126" t="s">
-        <v>66</v>
+    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="158"/>
+      <c r="B52" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C52" s="56" t="s">
         <v>15</v>
@@ -3194,9 +3186,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="156"/>
-      <c r="B53" s="127"/>
+    <row r="53" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="158"/>
+      <c r="B53" s="128"/>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
@@ -3212,9 +3204,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="156"/>
-      <c r="B54" s="127"/>
+    <row r="54" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="158"/>
+      <c r="B54" s="128"/>
       <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
@@ -3230,9 +3222,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="156"/>
-      <c r="B55" s="127"/>
+    <row r="55" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="158"/>
+      <c r="B55" s="128"/>
       <c r="C55" s="2" t="s">
         <v>6</v>
       </c>
@@ -3248,9 +3240,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="156"/>
-      <c r="B56" s="127"/>
+    <row r="56" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="158"/>
+      <c r="B56" s="128"/>
       <c r="C56" s="2" t="s">
         <v>7</v>
       </c>
@@ -3266,11 +3258,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="156"/>
-      <c r="B57" s="127"/>
+    <row r="57" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="158"/>
+      <c r="B57" s="128"/>
       <c r="C57" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D57" s="23"/>
       <c r="E57" s="23"/>
@@ -3284,9 +3276,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="156"/>
-      <c r="B58" s="127"/>
+    <row r="58" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="158"/>
+      <c r="B58" s="128"/>
       <c r="C58" s="2" t="s">
         <v>8</v>
       </c>
@@ -3302,8 +3294,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="156"/>
+    <row r="59" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="158"/>
       <c r="B59" s="5"/>
       <c r="C59" s="6" t="s">
         <v>9</v>
@@ -3341,28 +3333,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="157" t="s">
+    <row r="61" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="148" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="145" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="146"/>
-      <c r="D61" s="147"/>
-      <c r="E61" s="147"/>
-      <c r="F61" s="147"/>
-      <c r="G61" s="147"/>
-      <c r="H61" s="147"/>
-      <c r="I61" s="147"/>
-      <c r="J61" s="147"/>
-      <c r="K61" s="148"/>
-    </row>
-    <row r="62" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="157"/>
+      <c r="C61" s="140"/>
+      <c r="D61" s="141"/>
+      <c r="E61" s="141"/>
+      <c r="F61" s="141"/>
+      <c r="G61" s="141"/>
+      <c r="H61" s="141"/>
+      <c r="I61" s="141"/>
+      <c r="J61" s="141"/>
+      <c r="K61" s="142"/>
+    </row>
+    <row r="62" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="148"/>
       <c r="C62" s="1"/>
       <c r="D62" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E62" s="134"/>
       <c r="F62" s="134"/>
@@ -3372,8 +3364,8 @@
       <c r="J62" s="134"/>
       <c r="K62" s="47"/>
     </row>
-    <row r="63" spans="1:11" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A63" s="157"/>
+    <row r="63" spans="1:11" s="48" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="148"/>
       <c r="D63" s="58" t="s">
         <v>15</v>
       </c>
@@ -3390,7 +3382,7 @@
         <v>7</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J63" s="7" t="s">
         <v>8</v>
@@ -3399,10 +3391,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="157"/>
-      <c r="B64" s="126" t="s">
-        <v>66</v>
+    <row r="64" spans="1:11" s="48" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="148"/>
+      <c r="B64" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C64" s="56" t="s">
         <v>15</v>
@@ -3419,9 +3411,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="157"/>
-      <c r="B65" s="127"/>
+    <row r="65" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="148"/>
+      <c r="B65" s="128"/>
       <c r="C65" s="2" t="s">
         <v>4</v>
       </c>
@@ -3437,9 +3429,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="157"/>
-      <c r="B66" s="127"/>
+    <row r="66" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="148"/>
+      <c r="B66" s="128"/>
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
@@ -3455,9 +3447,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="157"/>
-      <c r="B67" s="127"/>
+    <row r="67" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="148"/>
+      <c r="B67" s="128"/>
       <c r="C67" s="2" t="s">
         <v>6</v>
       </c>
@@ -3473,9 +3465,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="157"/>
-      <c r="B68" s="127"/>
+    <row r="68" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="148"/>
+      <c r="B68" s="128"/>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
@@ -3491,11 +3483,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="157"/>
-      <c r="B69" s="127"/>
+    <row r="69" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="148"/>
+      <c r="B69" s="128"/>
       <c r="C69" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D69" s="23"/>
       <c r="E69" s="23"/>
@@ -3509,9 +3501,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="157"/>
-      <c r="B70" s="127"/>
+    <row r="70" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="148"/>
+      <c r="B70" s="128"/>
       <c r="C70" s="2" t="s">
         <v>8</v>
       </c>
@@ -3527,8 +3519,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="157"/>
+    <row r="71" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="148"/>
       <c r="B71" s="5"/>
       <c r="C71" s="6" t="s">
         <v>9</v>
@@ -3566,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="65"/>
       <c r="D72" s="46"/>
       <c r="E72" s="46"/>
@@ -3577,28 +3569,28 @@
       <c r="J72" s="46"/>
       <c r="K72" s="47"/>
     </row>
-    <row r="73" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="158" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" s="149" t="s">
-        <v>58</v>
-      </c>
-      <c r="C73" s="150"/>
-      <c r="D73" s="151"/>
-      <c r="E73" s="151"/>
-      <c r="F73" s="151"/>
-      <c r="G73" s="151"/>
-      <c r="H73" s="151"/>
-      <c r="I73" s="151"/>
-      <c r="J73" s="151"/>
-      <c r="K73" s="152"/>
-    </row>
-    <row r="74" spans="1:11" s="48" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="158"/>
+    <row r="73" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="149" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="143" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="144"/>
+      <c r="D73" s="145"/>
+      <c r="E73" s="145"/>
+      <c r="F73" s="145"/>
+      <c r="G73" s="145"/>
+      <c r="H73" s="145"/>
+      <c r="I73" s="145"/>
+      <c r="J73" s="145"/>
+      <c r="K73" s="146"/>
+    </row>
+    <row r="74" spans="1:11" s="48" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="149"/>
       <c r="C74" s="1"/>
       <c r="D74" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E74" s="134"/>
       <c r="F74" s="134"/>
@@ -3608,8 +3600,8 @@
       <c r="J74" s="134"/>
       <c r="K74" s="47"/>
     </row>
-    <row r="75" spans="1:11" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A75" s="158"/>
+    <row r="75" spans="1:11" s="48" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="149"/>
       <c r="D75" s="58" t="s">
         <v>15</v>
       </c>
@@ -3626,7 +3618,7 @@
         <v>7</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J75" s="7" t="s">
         <v>8</v>
@@ -3635,10 +3627,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A76" s="158"/>
-      <c r="B76" s="126" t="s">
-        <v>66</v>
+    <row r="76" spans="1:11" s="48" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="149"/>
+      <c r="B76" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C76" s="56" t="s">
         <v>15</v>
@@ -3655,9 +3647,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="158"/>
-      <c r="B77" s="127"/>
+    <row r="77" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="149"/>
+      <c r="B77" s="128"/>
       <c r="C77" s="2" t="s">
         <v>4</v>
       </c>
@@ -3673,9 +3665,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="158"/>
-      <c r="B78" s="127"/>
+    <row r="78" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="149"/>
+      <c r="B78" s="128"/>
       <c r="C78" s="2" t="s">
         <v>5</v>
       </c>
@@ -3691,9 +3683,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="158"/>
-      <c r="B79" s="127"/>
+    <row r="79" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="149"/>
+      <c r="B79" s="128"/>
       <c r="C79" s="2" t="s">
         <v>6</v>
       </c>
@@ -3709,9 +3701,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="158"/>
-      <c r="B80" s="127"/>
+    <row r="80" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="149"/>
+      <c r="B80" s="128"/>
       <c r="C80" s="2" t="s">
         <v>7</v>
       </c>
@@ -3727,11 +3719,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="158"/>
-      <c r="B81" s="127"/>
+    <row r="81" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="149"/>
+      <c r="B81" s="128"/>
       <c r="C81" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="23"/>
@@ -3745,9 +3737,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="158"/>
-      <c r="B82" s="127"/>
+    <row r="82" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="149"/>
+      <c r="B82" s="128"/>
       <c r="C82" s="2" t="s">
         <v>8</v>
       </c>
@@ -3763,8 +3755,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="158"/>
+    <row r="83" spans="1:11" s="48" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="149"/>
       <c r="B83" s="5"/>
       <c r="C83" s="6" t="s">
         <v>9</v>
@@ -3802,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="65"/>
       <c r="D84" s="46"/>
       <c r="E84" s="46"/>
@@ -3813,28 +3805,28 @@
       <c r="J84" s="46"/>
       <c r="K84" s="47"/>
     </row>
-    <row r="85" spans="1:11" s="61" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="159" t="s">
+    <row r="85" spans="1:11" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="153" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" s="153"/>
-      <c r="D85" s="153"/>
-      <c r="E85" s="153"/>
-      <c r="F85" s="153"/>
-      <c r="G85" s="153"/>
-      <c r="H85" s="153"/>
-      <c r="I85" s="153"/>
-      <c r="J85" s="153"/>
-      <c r="K85" s="153"/>
-    </row>
-    <row r="86" spans="1:11" s="61" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="159"/>
+      <c r="B85" s="159" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" s="159"/>
+      <c r="D85" s="159"/>
+      <c r="E85" s="159"/>
+      <c r="F85" s="159"/>
+      <c r="G85" s="159"/>
+      <c r="H85" s="159"/>
+      <c r="I85" s="159"/>
+      <c r="J85" s="159"/>
+      <c r="K85" s="159"/>
+    </row>
+    <row r="86" spans="1:11" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="150"/>
       <c r="C86" s="1"/>
       <c r="D86" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E86" s="134"/>
       <c r="F86" s="134"/>
@@ -3844,8 +3836,8 @@
       <c r="J86" s="134"/>
       <c r="K86" s="63"/>
     </row>
-    <row r="87" spans="1:11" s="61" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A87" s="159"/>
+    <row r="87" spans="1:11" s="61" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="150"/>
       <c r="D87" s="58" t="s">
         <v>15</v>
       </c>
@@ -3862,7 +3854,7 @@
         <v>7</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J87" s="7" t="s">
         <v>8</v>
@@ -3871,10 +3863,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="61" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A88" s="159"/>
-      <c r="B88" s="126" t="s">
-        <v>66</v>
+    <row r="88" spans="1:11" s="61" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="150"/>
+      <c r="B88" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C88" s="56" t="s">
         <v>15</v>
@@ -3891,9 +3883,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="159"/>
-      <c r="B89" s="127"/>
+    <row r="89" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="150"/>
+      <c r="B89" s="128"/>
       <c r="C89" s="2" t="s">
         <v>4</v>
       </c>
@@ -3909,9 +3901,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="159"/>
-      <c r="B90" s="127"/>
+    <row r="90" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="150"/>
+      <c r="B90" s="128"/>
       <c r="C90" s="2" t="s">
         <v>5</v>
       </c>
@@ -3927,9 +3919,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="159"/>
-      <c r="B91" s="127"/>
+    <row r="91" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="150"/>
+      <c r="B91" s="128"/>
       <c r="C91" s="2" t="s">
         <v>6</v>
       </c>
@@ -3945,9 +3937,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="159"/>
-      <c r="B92" s="127"/>
+    <row r="92" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="150"/>
+      <c r="B92" s="128"/>
       <c r="C92" s="2" t="s">
         <v>7</v>
       </c>
@@ -3963,11 +3955,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="159"/>
-      <c r="B93" s="127"/>
+    <row r="93" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="150"/>
+      <c r="B93" s="128"/>
       <c r="C93" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D93" s="23"/>
       <c r="E93" s="23"/>
@@ -3981,9 +3973,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="159"/>
-      <c r="B94" s="127"/>
+    <row r="94" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="150"/>
+      <c r="B94" s="128"/>
       <c r="C94" s="2" t="s">
         <v>8</v>
       </c>
@@ -3999,8 +3991,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="159"/>
+    <row r="95" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="150"/>
       <c r="B95" s="5"/>
       <c r="C95" s="6" t="s">
         <v>9</v>
@@ -4038,28 +4030,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="61" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="154" t="s">
+    <row r="97" spans="1:11" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="B97" s="132" t="s">
-        <v>41</v>
-      </c>
-      <c r="C97" s="132"/>
-      <c r="D97" s="132"/>
-      <c r="E97" s="132"/>
-      <c r="F97" s="132"/>
-      <c r="G97" s="132"/>
-      <c r="H97" s="132"/>
-      <c r="I97" s="132"/>
-      <c r="J97" s="132"/>
-      <c r="K97" s="132"/>
-    </row>
-    <row r="98" spans="1:11" s="61" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="154"/>
+      <c r="B97" s="154" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97" s="154"/>
+      <c r="D97" s="154"/>
+      <c r="E97" s="154"/>
+      <c r="F97" s="154"/>
+      <c r="G97" s="154"/>
+      <c r="H97" s="154"/>
+      <c r="I97" s="154"/>
+      <c r="J97" s="154"/>
+      <c r="K97" s="154"/>
+    </row>
+    <row r="98" spans="1:11" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="156"/>
       <c r="C98" s="1"/>
       <c r="D98" s="133" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E98" s="134"/>
       <c r="F98" s="134"/>
@@ -4069,8 +4061,8 @@
       <c r="J98" s="134"/>
       <c r="K98" s="63"/>
     </row>
-    <row r="99" spans="1:11" s="61" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A99" s="154"/>
+    <row r="99" spans="1:11" s="61" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A99" s="156"/>
       <c r="D99" s="58" t="s">
         <v>15</v>
       </c>
@@ -4087,7 +4079,7 @@
         <v>7</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J99" s="7" t="s">
         <v>8</v>
@@ -4096,10 +4088,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="61" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A100" s="154"/>
-      <c r="B100" s="126" t="s">
-        <v>66</v>
+    <row r="100" spans="1:11" s="61" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="156"/>
+      <c r="B100" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="C100" s="56" t="s">
         <v>15</v>
@@ -4116,9 +4108,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A101" s="154"/>
-      <c r="B101" s="127"/>
+    <row r="101" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="156"/>
+      <c r="B101" s="128"/>
       <c r="C101" s="2" t="s">
         <v>4</v>
       </c>
@@ -4134,9 +4126,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="154"/>
-      <c r="B102" s="127"/>
+    <row r="102" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="156"/>
+      <c r="B102" s="128"/>
       <c r="C102" s="2" t="s">
         <v>5</v>
       </c>
@@ -4152,9 +4144,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="154"/>
-      <c r="B103" s="127"/>
+    <row r="103" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="156"/>
+      <c r="B103" s="128"/>
       <c r="C103" s="2" t="s">
         <v>6</v>
       </c>
@@ -4170,9 +4162,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="154"/>
-      <c r="B104" s="127"/>
+    <row r="104" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="156"/>
+      <c r="B104" s="128"/>
       <c r="C104" s="2" t="s">
         <v>7</v>
       </c>
@@ -4188,11 +4180,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="154"/>
-      <c r="B105" s="127"/>
+    <row r="105" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="156"/>
+      <c r="B105" s="128"/>
       <c r="C105" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D105" s="23"/>
       <c r="E105" s="23"/>
@@ -4206,9 +4198,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A106" s="154"/>
-      <c r="B106" s="127"/>
+    <row r="106" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="156"/>
+      <c r="B106" s="128"/>
       <c r="C106" s="2" t="s">
         <v>8</v>
       </c>
@@ -4224,8 +4216,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="154"/>
+    <row r="107" spans="1:11" s="61" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="156"/>
       <c r="B107" s="5"/>
       <c r="C107" s="6" t="s">
         <v>9</v>
@@ -4263,28 +4255,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:11" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="66"/>
-      <c r="B118" s="107" t="s">
+      <c r="B118" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="136"/>
-      <c r="D118" s="136"/>
-      <c r="E118" s="136"/>
-      <c r="F118" s="136"/>
-      <c r="G118" s="136"/>
-      <c r="H118" s="136"/>
-      <c r="I118" s="136"/>
-      <c r="J118" s="136"/>
-      <c r="K118" s="136"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C118" s="126"/>
+      <c r="D118" s="126"/>
+      <c r="E118" s="126"/>
+      <c r="F118" s="126"/>
+      <c r="G118" s="126"/>
+      <c r="H118" s="126"/>
+      <c r="I118" s="126"/>
+      <c r="J118" s="126"/>
+      <c r="K118" s="126"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B120" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B88:B94"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A97:A107"/>
+    <mergeCell ref="A37:A47"/>
+    <mergeCell ref="A49:A59"/>
+    <mergeCell ref="B85:K85"/>
+    <mergeCell ref="D86:J86"/>
+    <mergeCell ref="D98:J98"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B52:B58"/>
     <mergeCell ref="A61:A71"/>
     <mergeCell ref="A73:A83"/>
     <mergeCell ref="A85:A95"/>
@@ -4301,25 +4311,7 @@
     <mergeCell ref="B73:K73"/>
     <mergeCell ref="D74:J74"/>
     <mergeCell ref="B76:B82"/>
-    <mergeCell ref="B85:K85"/>
-    <mergeCell ref="D86:J86"/>
-    <mergeCell ref="D98:J98"/>
     <mergeCell ref="B100:B106"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B88:B94"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B25:K25"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A97:A107"/>
-    <mergeCell ref="A37:A47"/>
-    <mergeCell ref="A49:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4330,53 +4322,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" style="34"/>
-    <col min="2" max="2" width="14.53125" style="34" customWidth="1"/>
-    <col min="3" max="10" width="15.53125" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="9.19921875" style="34"/>
+    <col min="1" max="1" width="9.21875" style="34"/>
+    <col min="2" max="2" width="14.5546875" style="34" customWidth="1"/>
+    <col min="3" max="10" width="15.5546875" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="9.21875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="161" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-    </row>
-    <row r="4" spans="1:10" ht="29.25" x14ac:dyDescent="0.55000000000000004">
+        <v>58</v>
+      </c>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+    </row>
+    <row r="4" spans="1:10" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="F4" s="42" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
       <c r="E5" s="28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="40">
         <f>SUM(F6:F9)</f>
@@ -4390,12 +4384,12 @@
       <c r="I5" s="35"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
       <c r="E6" s="28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="49"/>
       <c r="G6" s="50" t="e">
@@ -4406,12 +4400,12 @@
       <c r="I6" s="35"/>
       <c r="J6" s="36"/>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
       <c r="E7" s="28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="29" t="e">
@@ -4422,12 +4416,12 @@
       <c r="I7" s="35"/>
       <c r="J7" s="36"/>
     </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="53"/>
       <c r="G8" s="54" t="e">
@@ -4438,12 +4432,12 @@
       <c r="I8" s="35"/>
       <c r="J8" s="36"/>
     </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="52" t="e">
@@ -4454,25 +4448,25 @@
       <c r="I9" s="35"/>
       <c r="J9" s="36"/>
     </row>
-    <row r="10" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="F11" s="27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G11" s="31" t="e">
         <f>I22/G22</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="162" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B13" s="163"/>
       <c r="C13" s="163"/>
@@ -4484,36 +4478,36 @@
       <c r="I13" s="163"/>
       <c r="J13" s="163"/>
     </row>
-    <row r="14" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="G15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="I15" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="164"/>
       <c r="B16" s="56" t="s">
         <v>15</v>
@@ -4539,8 +4533,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="127"/>
+    <row r="17" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="128"/>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4565,8 +4559,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="127"/>
+    <row r="18" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="128"/>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -4591,8 +4585,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="127"/>
+    <row r="19" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="128"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -4617,8 +4611,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="127"/>
+    <row r="20" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="128"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -4643,10 +4637,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="127"/>
+    <row r="21" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="128"/>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -4669,7 +4663,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="C22" s="25"/>
       <c r="D22" s="6" t="s">
@@ -4696,34 +4690,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="165" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="127"/>
-      <c r="C24" s="127"/>
-      <c r="D24" s="127"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
-      <c r="G24" s="127"/>
-      <c r="H24" s="127"/>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>71</v>
+      </c>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="166" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="127"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
-      <c r="G25" s="127"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-    </row>
-    <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C26" s="32" t="s">
         <v>15</v>
       </c>
@@ -4740,12 +4734,12 @@
         <v>7</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="164" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B27" s="56" t="s">
         <v>15</v>
@@ -4757,7 +4751,7 @@
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
     </row>
-    <row r="28" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="164"/>
       <c r="B28" s="2" t="s">
         <v>4</v>
@@ -4769,7 +4763,7 @@
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
     </row>
-    <row r="29" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="164"/>
       <c r="B29" s="2" t="s">
         <v>5</v>
@@ -4781,7 +4775,7 @@
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
     </row>
-    <row r="30" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="164"/>
       <c r="B30" s="2" t="s">
         <v>6</v>
@@ -4793,7 +4787,7 @@
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="164"/>
       <c r="B31" s="2" t="s">
         <v>7</v>
@@ -4805,10 +4799,10 @@
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="164"/>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
@@ -4817,7 +4811,7 @@
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
     </row>
-    <row r="33" spans="1:10" s="38" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" s="38" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="6"/>
       <c r="C33" s="45"/>
@@ -4829,9 +4823,9 @@
       <c r="I33" s="36"/>
       <c r="J33" s="36"/>
     </row>
-    <row r="34" spans="1:10" s="38" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="105" t="s">
-        <v>73</v>
+    <row r="34" spans="1:10" s="38" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="122" t="s">
+        <v>69</v>
       </c>
       <c r="B34" s="160"/>
       <c r="C34" s="160"/>
@@ -4843,24 +4837,22 @@
       <c r="I34" s="160"/>
       <c r="J34" s="160"/>
     </row>
-    <row r="36" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="107" t="s">
+    <row r="36" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="136"/>
-      <c r="F36" s="136"/>
-      <c r="G36" s="136"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A38" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="126"/>
+      <c r="H36" s="126"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="126"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="33"/>
       <c r="C38" s="35"/>
       <c r="D38" s="35"/>
       <c r="E38" s="35"/>
@@ -4890,55 +4882,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" style="34" customWidth="1"/>
-    <col min="2" max="2" width="14.53125" style="34" customWidth="1"/>
-    <col min="3" max="9" width="15.53125" style="34" customWidth="1"/>
-    <col min="10" max="10" width="15.53125" style="36" customWidth="1"/>
-    <col min="11" max="16384" width="9.19921875" style="34"/>
+    <col min="1" max="1" width="8.77734375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="34" customWidth="1"/>
+    <col min="3" max="9" width="15.5546875" style="34" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="36" customWidth="1"/>
+    <col min="11" max="16384" width="9.21875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="161" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
+        <v>59</v>
+      </c>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="167"/>
     </row>
-    <row r="4" spans="1:10" ht="29.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="F4" s="42" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
       <c r="E5" s="28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="40">
         <f>SUM(F6:F9)</f>
@@ -4951,12 +4945,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
       <c r="E6" s="28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="49"/>
       <c r="G6" s="50" t="e">
@@ -4966,12 +4960,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
       <c r="E7" s="28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="29" t="e">
@@ -4981,12 +4975,12 @@
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
     </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F8" s="53"/>
       <c r="G8" s="54" t="e">
@@ -4996,12 +4990,12 @@
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="52" t="e">
@@ -5011,13 +5005,13 @@
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
     </row>
-    <row r="10" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="J10" s="34"/>
     </row>
-    <row r="11" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="168" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" s="169"/>
       <c r="C11" s="169"/>
@@ -5029,16 +5023,16 @@
       <c r="I11" s="169"/>
       <c r="J11" s="170"/>
     </row>
-    <row r="12" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>12</v>
@@ -5047,7 +5041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="164"/>
       <c r="B14" s="56" t="s">
         <v>15</v>
@@ -5069,8 +5063,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="127"/>
+    <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="128"/>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
@@ -5091,8 +5085,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="127"/>
+    <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="128"/>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -5113,8 +5107,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="127"/>
+    <row r="17" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="128"/>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -5135,8 +5129,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="127"/>
+    <row r="18" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="128"/>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -5157,10 +5151,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="127"/>
+    <row r="19" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="128"/>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19" s="23">
         <f t="shared" si="1"/>
@@ -5179,8 +5173,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="127"/>
+    <row r="20" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="128"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -5201,7 +5195,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="6" t="s">
         <v>9</v>
@@ -5220,30 +5214,30 @@
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:10" ht="18.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
     </row>
-    <row r="23" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="127"/>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="127"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
       <c r="J23" s="167"/>
     </row>
-    <row r="24" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="166" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D24" s="166"/>
       <c r="E24" s="166"/>
@@ -5253,7 +5247,7 @@
       <c r="I24" s="166"/>
       <c r="J24" s="68"/>
     </row>
-    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C25" s="57" t="s">
         <v>15</v>
       </c>
@@ -5270,7 +5264,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>8</v>
@@ -5279,9 +5273,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="126" t="s">
-        <v>66</v>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="127" t="s">
+        <v>62</v>
       </c>
       <c r="B26" s="56" t="s">
         <v>15</v>
@@ -5298,8 +5292,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="127"/>
+    <row r="27" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="128"/>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
@@ -5315,8 +5309,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="127"/>
+    <row r="28" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="128"/>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
@@ -5332,8 +5326,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="127"/>
+    <row r="29" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="128"/>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -5349,8 +5343,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="127"/>
+    <row r="30" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="128"/>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
@@ -5366,10 +5360,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="127"/>
+    <row r="31" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="128"/>
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
@@ -5383,8 +5377,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="127"/>
+    <row r="32" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="128"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5400,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="38" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" s="38" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="6" t="s">
         <v>9</v>
@@ -5438,24 +5432,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="107" t="s">
+    <row r="35" spans="1:10" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="136"/>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="136"/>
-      <c r="G35" s="136"/>
-      <c r="H35" s="136"/>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="126"/>
+      <c r="H35" s="126"/>
+      <c r="I35" s="126"/>
+      <c r="J35" s="126"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="33"/>
       <c r="C37" s="35"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>

</xml_diff>